<commit_message>
update Param.xlsx: add parameters of interest
</commit_message>
<xml_diff>
--- a/InSilicoBottomUp_Workshop/Param.xlsx
+++ b/InSilicoBottomUp_Workshop/Param.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpk349/Documents/Boulot/GitRepo/InSilicoWorkshop/ForWorkshop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpk349/Documents/Boulot/GitRepo/InSilicoWorkshop/InSilicoBottomUp_Workshop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A5571698-98C7-744B-B3DA-895F9714FAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DADF636-EC3C-A846-94D5-6AC1696BB86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Param" sheetId="1" r:id="rId1"/>
+    <sheet name="Parameters of interest" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Param!$A$1:$S$31</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="54">
   <si>
     <t>PathToFasta</t>
   </si>
@@ -152,13 +153,136 @@
   </si>
   <si>
     <t>../Output/UPS1-like_output/outputMSRun_f692c5374fb95f1cfcda33125af91bc1.RData</t>
+  </si>
+  <si>
+    <t>full_yeast</t>
+  </si>
+  <si>
+    <r>
+      <t>2,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft New Tai Lue"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft New Tai Lue"/>
+      </rPr>
+      <t>,4,5,6</t>
+    </r>
+  </si>
+  <si>
+    <t>NumCond</t>
+  </si>
+  <si>
+    <r>
+      <t>0.01,0.125,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft New Tai Lue"/>
+      </rPr>
+      <t>0.25</t>
+    </r>
+  </si>
+  <si>
+    <t>DiffRegFrac</t>
+  </si>
+  <si>
+    <t>DiffRegMax</t>
+  </si>
+  <si>
+    <r>
+      <t>trypsin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft New Tai Lue"/>
+      </rPr>
+      <t>, trypsin.strict</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft New Tai Lue"/>
+      </rPr>
+      <t>,0.1,0.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.1,0.25,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft New Tai Lue"/>
+      </rPr>
+      <t>0.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.01,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft New Tai Lue"/>
+      </rPr>
+      <t>0.125</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft New Tai Lue"/>
+      </rPr>
+      <t>,0.25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft New Tai Lue"/>
+      </rPr>
+      <t>,0.05</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -293,8 +417,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft New Tai Lue"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft New Tai Lue"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,8 +609,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C9CA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -590,6 +737,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA31D20"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFA31D20"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFA31D20"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFA31D20"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA31D20"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFA31D20"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -635,8 +808,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -991,10 +1173,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1996,7 +2178,118 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S31"/>
+  <autoFilter ref="A1:S31" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE91AE8-CC88-6F4D-9A23-8B28FD8B6BC5}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="78.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="31" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>